<commit_message>
Fixed main radial field macro
</commit_message>
<xml_diff>
--- a/RadialFieldOps/RadialFieldScan.xlsx
+++ b/RadialFieldOps/RadialFieldScan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/RadialFieldOps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9743DC18-2094-E24A-8CB0-EBA2D7EA4E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1E0DC0-BFDF-B347-B822-2114648494E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
+    <workbookView xWindow="-3400" yWindow="-18540" windowWidth="17780" windowHeight="16540" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1509,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B752E6E-F960-2F47-AC55-2B0104D935A3}">
-  <dimension ref="A2:K11"/>
+  <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1777,6 +1777,12 @@
         <v>16</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J14" s="2">
+        <f>AVERAGE(J5,J6,J10,J11)</f>
+        <v>2864755.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>